<commit_message>
Added more error checking and exception handling
</commit_message>
<xml_diff>
--- a/InstallIssues.xlsx
+++ b/InstallIssues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankserrao/MyStuff/TestAndPlay/Click2Mail/generative-ai-marketing-portal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankserrao/MyStuff/TestAndPlay/Click2Mail/c2m-generative-ai-marketing-portal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F120F9C-6961-4941-9BD0-5F807C97D325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544ED604-7236-2842-8DEA-DE9E5B296CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{65CAFB45-5EA5-CC4E-84F7-FBFAC622A23F}"/>
   </bookViews>
@@ -896,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26BA907-60B3-4449-9748-331EA4B9C82B}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,11 +1079,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="404" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="13" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Formatting and freezing poetry version of python
</commit_message>
<xml_diff>
--- a/InstallIssues.xlsx
+++ b/InstallIssues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankserrao/MyStuff/TestAndPlay/Click2Mail/c2m-generative-ai-marketing-portal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544ED604-7236-2842-8DEA-DE9E5B296CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CBDA4F-4512-4940-BEC2-198AD0CEBE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{65CAFB45-5EA5-CC4E-84F7-FBFAC622A23F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>df_item_deduplicated_withPromotionFiledAdded.csv</t>
   </si>
@@ -268,12 +268,64 @@
   <si>
     <t>Needed to add langchain-community to the pyproject.toml file.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Issues identified but not fixed in the pull version </t>
+  </si>
+  <si>
+    <t>#15 [11/12] RUN poetry install --only main
+#15 2.487 The currently activated Python version 3.9.20 is not supported by the project (3.9.19).
+#15 2.487 Trying to find and use a compatible version. 
+#15 3.188 
+#15 3.188 Poetry was unable to find a compatible version. If you have one, you can explicitly use it via the "env use" command.
+#15 ERROR: process "/bin/sh -c poetry install --only main" did not complete successfully: exit code: 1</t>
+  </si>
+  <si>
+    <t>If the Dockerfile doesn’t specify an exact version (like 3.9.19), Docker will pull the latest version of the 3.9-slim image, which could be the reason for the unexpected change to Python 3.9.20.</t>
+  </si>
+  <si>
+    <t># Copyright 2023 Amazon.com, Inc. or its affiliates. All Rights Reserved.
+#
+# This is AWS Content subject to the terms of the Customer Agreement
+# ----------------------------------------------------------------------
+# File content:
+#       Docker image of the streamlit container
+FROM --platform=linux/amd64 python:3.9.19-slim
+WORKDIR /app
+RUN apt-get update -y &amp;&amp; apt-get install -y --no-install-recommends\
+    build-essential \
+    curl \
+    software-properties-common \
+    git \
+    &amp;&amp; rm -rf /var/lib/apt/lists/*
+COPY streamlit/pyproject.toml /app
+COPY streamlit/.streamlit/ /app/.streamlit/
+COPY shared_module/python /app/shared_module
+RUN python --version
+RUN pip3 --no-cache-dir install -U pip
+RUN pip3 --no-cache-dir install poetry
+RUN poetry config virtualenvs.create false
+RUN poetry install --only main
+COPY streamlit/src/ /app/src
+EXPOSE 8501
+HEALTHCHECK CMD curl --fail http://localhost:8501/_stcore/health
+ENTRYPOINT ["streamlit", "run", "src/Home.py", "--server.port=8501", "--server.address=0.0.0.0"]</t>
+  </si>
+  <si>
+    <t>Find and Pin a Specific Version of the Docker Image
+To ensure stability, you should pin the Docker image to a specific version. Here's how:
+Check Docker Hub: You can go to the official Python Docker Hub page and search for the specific version tags. For example, if you want Python 3.9.19, look for a tag like python:3.9.19-slim.
+Pin the Version in the Dockerfile: Once you've identified the version that worked for you (e.g., 3.9.19), modify your Dockerfile to pin that specific version.
+For example, if 3.9.19-slim was working for you:
+Dockerfile
+Copy code
+FROM python:3.9.19-slim</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -304,13 +356,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -340,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -356,6 +427,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26BA907-60B3-4449-9748-331EA4B9C82B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,7 +1167,39 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:E14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>